<commit_message>
Excel to txt seems to be working.
</commit_message>
<xml_diff>
--- a/tests/sample_files/entity_dictionaries/foo.xlsx
+++ b/tests/sample_files/entity_dictionaries/foo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="5850" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>authority</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>foo.mixed</t>
+  </si>
+  <si>
+    <t>Lorem ...</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +419,9 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
@@ -430,6 +436,9 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
@@ -443,6 +452,9 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Adding wildcard support; added examples to Excel file.
</commit_message>
<xml_diff>
--- a/tests/sample_files/entity_dictionaries/foo.xlsx
+++ b/tests/sample_files/entity_dictionaries/foo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>authority</t>
   </si>
@@ -58,6 +58,27 @@
   </si>
   <si>
     <t>Lorem ...</t>
+  </si>
+  <si>
+    <t>bar {abc}Bar</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>bar{abc} Bar</t>
+  </si>
+  <si>
+    <t>{123}</t>
+  </si>
+  <si>
+    <t>{123} {abc}</t>
+  </si>
+  <si>
+    <t>foo {abc} bar</t>
   </si>
 </sst>
 </file>
@@ -384,15 +405,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -466,6 +488,91 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>